<commit_message>
Feat: add AUS data
Add the folder of AUS raw data files and the notebook to clean the data and generate the xlsx spreadsheet for the scripts to read in.
</commit_message>
<xml_diff>
--- a/data/quarterly_data_AUS.xlsx
+++ b/data/quarterly_data_AUS.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,25 +456,30 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>domestic_final_demand_index</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>2yr_govt_bond_yield_qrtly</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>3yr_bond_spread_qrtly</t>
+          <t>3yr_credit_spread_qrtly</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>house_price_index</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>rent_index</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>home_ownership_pct</t>
         </is>
@@ -494,18 +499,21 @@
         <v>65.40000000000001</v>
       </c>
       <c r="E2" t="n">
+        <v>69</v>
+      </c>
+      <c r="F2" t="n">
         <v>5.365000417710942</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>0.7569933166248962</v>
       </c>
-      <c r="G2" t="n">
+      <c r="H2" t="n">
         <v>81.3168</v>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>70.90000000000001</v>
       </c>
-      <c r="I2" t="n">
+      <c r="J2" t="n">
         <v>69.3</v>
       </c>
     </row>
@@ -523,18 +531,21 @@
         <v>66.3</v>
       </c>
       <c r="E3" t="n">
+        <v>69.3</v>
+      </c>
+      <c r="F3" t="n">
         <v>5.258725108225108</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>0.5857691197691194</v>
       </c>
-      <c r="G3" t="n">
+      <c r="H3" t="n">
         <v>80.4252</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>71.40000000000001</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
         <v>69.3</v>
       </c>
     </row>
@@ -552,18 +563,21 @@
         <v>65.8</v>
       </c>
       <c r="E4" t="n">
+        <v>70</v>
+      </c>
+      <c r="F4" t="n">
         <v>5.156752933057281</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>0.6573080180688867</v>
       </c>
-      <c r="G4" t="n">
+      <c r="H4" t="n">
         <v>81.5955</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>71.8</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
         <v>69.3</v>
       </c>
     </row>
@@ -581,18 +595,21 @@
         <v>65.59999999999999</v>
       </c>
       <c r="E5" t="n">
+        <v>70.5</v>
+      </c>
+      <c r="F5" t="n">
         <v>5.299302308802308</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>0.6183225108225102</v>
       </c>
-      <c r="G5" t="n">
+      <c r="H5" t="n">
         <v>81.8004</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>72.3</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
         <v>69.3</v>
       </c>
     </row>
@@ -610,18 +627,21 @@
         <v>65.09999999999999</v>
       </c>
       <c r="E6" t="n">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="F6" t="n">
         <v>5.23088768115942</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>0.6912246376811592</v>
       </c>
-      <c r="G6" t="n">
+      <c r="H6" t="n">
         <v>83.3913</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>72.90000000000001</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -639,18 +659,21 @@
         <v>66.09999999999999</v>
       </c>
       <c r="E7" t="n">
+        <v>71.90000000000001</v>
+      </c>
+      <c r="F7" t="n">
         <v>5.650908334348233</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>0.7360094182600569</v>
       </c>
-      <c r="G7" t="n">
+      <c r="H7" t="n">
         <v>84.124</v>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>73.5</v>
       </c>
-      <c r="I7" t="n">
+      <c r="J7" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -668,18 +691,21 @@
         <v>68.09999999999999</v>
       </c>
       <c r="E8" t="n">
+        <v>72.59999999999999</v>
+      </c>
+      <c r="F8" t="n">
         <v>5.908381642512079</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>0.6650966183574883</v>
       </c>
-      <c r="G8" t="n">
+      <c r="H8" t="n">
         <v>85.7251</v>
       </c>
-      <c r="H8" t="n">
+      <c r="I8" t="n">
         <v>74.3</v>
       </c>
-      <c r="I8" t="n">
+      <c r="J8" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -697,18 +723,21 @@
         <v>69.40000000000001</v>
       </c>
       <c r="E9" t="n">
+        <v>73</v>
+      </c>
+      <c r="F9" t="n">
         <v>6.027666514771777</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>0.7225774663932562</v>
       </c>
-      <c r="G9" t="n">
+      <c r="H9" t="n">
         <v>86.47709999999999</v>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>75</v>
       </c>
-      <c r="I9" t="n">
+      <c r="J9" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -726,18 +755,21 @@
         <v>69.40000000000001</v>
       </c>
       <c r="E10" t="n">
+        <v>73.3</v>
+      </c>
+      <c r="F10" t="n">
         <v>6.125588023088024</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>0.6631562049062047</v>
       </c>
-      <c r="G10" t="n">
+      <c r="H10" t="n">
         <v>89.21120000000001</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>76.09999999999999</v>
       </c>
-      <c r="I10" t="n">
+      <c r="J10" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -755,18 +787,21 @@
         <v>69.40000000000001</v>
       </c>
       <c r="E11" t="n">
+        <v>73.90000000000001</v>
+      </c>
+      <c r="F11" t="n">
         <v>6.281530998389695</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>0.6827516103059574</v>
       </c>
-      <c r="G11" t="n">
+      <c r="H11" t="n">
         <v>91.7657</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>77.3</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -784,18 +819,21 @@
         <v>70.3</v>
       </c>
       <c r="E12" t="n">
+        <v>74.59999999999999</v>
+      </c>
+      <c r="F12" t="n">
         <v>6.332551834130782</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>0.8979106858054239</v>
       </c>
-      <c r="G12" t="n">
+      <c r="H12" t="n">
         <v>94.3873</v>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>78.59999999999999</v>
       </c>
-      <c r="I12" t="n">
+      <c r="J12" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -813,18 +851,21 @@
         <v>70.40000000000001</v>
       </c>
       <c r="E13" t="n">
+        <v>75.09999999999999</v>
+      </c>
+      <c r="F13" t="n">
         <v>6.653988280979128</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>1.357191248873171</v>
       </c>
-      <c r="G13" t="n">
+      <c r="H13" t="n">
         <v>93.54510000000001</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>80</v>
       </c>
-      <c r="I13" t="n">
+      <c r="J13" t="n">
         <v>68.3</v>
       </c>
     </row>
@@ -842,18 +883,21 @@
         <v>71.90000000000001</v>
       </c>
       <c r="E14" t="n">
+        <v>75.90000000000001</v>
+      </c>
+      <c r="F14" t="n">
         <v>6.576908939014203</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>2.019252297410192</v>
       </c>
-      <c r="G14" t="n">
+      <c r="H14" t="n">
         <v>91.405</v>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>81.40000000000001</v>
       </c>
-      <c r="I14" t="n">
+      <c r="J14" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -871,18 +915,21 @@
         <v>72.59999999999999</v>
       </c>
       <c r="E15" t="n">
+        <v>76.59999999999999</v>
+      </c>
+      <c r="F15" t="n">
         <v>6.633396464646464</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>2.143913059163058</v>
       </c>
-      <c r="G15" t="n">
+      <c r="H15" t="n">
         <v>88.3133</v>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>83.3</v>
       </c>
-      <c r="I15" t="n">
+      <c r="J15" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -900,18 +947,21 @@
         <v>73</v>
       </c>
       <c r="E16" t="n">
+        <v>77.8</v>
+      </c>
+      <c r="F16" t="n">
         <v>5.993195981554678</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1.988846179183136</v>
       </c>
-      <c r="G16" t="n">
+      <c r="H16" t="n">
         <v>87.3918</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>85</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -929,18 +979,21 @@
         <v>71.2</v>
       </c>
       <c r="E17" t="n">
+        <v>78.7</v>
+      </c>
+      <c r="F17" t="n">
         <v>3.6859613997114</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>3.39536075036075</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>87.0962</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>86.7</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -958,18 +1011,21 @@
         <v>70.8</v>
       </c>
       <c r="E18" t="n">
+        <v>79.2</v>
+      </c>
+      <c r="F18" t="n">
         <v>2.835189393939393</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>3.401848484848485</v>
       </c>
-      <c r="G18" t="n">
+      <c r="H18" t="n">
         <v>90.3262</v>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>88</v>
       </c>
-      <c r="I18" t="n">
+      <c r="J18" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -987,18 +1043,21 @@
         <v>71.2</v>
       </c>
       <c r="E19" t="n">
+        <v>79.3</v>
+      </c>
+      <c r="F19" t="n">
         <v>3.507769841269841</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>2.397984126984127</v>
       </c>
-      <c r="G19" t="n">
+      <c r="H19" t="n">
         <v>93.22839999999999</v>
       </c>
-      <c r="H19" t="n">
+      <c r="I19" t="n">
         <v>89.3</v>
       </c>
-      <c r="I19" t="n">
+      <c r="J19" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -1016,18 +1075,21 @@
         <v>72.3</v>
       </c>
       <c r="E20" t="n">
+        <v>79.7</v>
+      </c>
+      <c r="F20" t="n">
         <v>4.343870223978921</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>1.791221673254282</v>
       </c>
-      <c r="G20" t="n">
+      <c r="H20" t="n">
         <v>97.86399999999999</v>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>90.3</v>
       </c>
-      <c r="I20" t="n">
+      <c r="J20" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -1045,18 +1107,21 @@
         <v>74.40000000000001</v>
       </c>
       <c r="E21" t="n">
+        <v>79.90000000000001</v>
+      </c>
+      <c r="F21" t="n">
         <v>4.69063492063492</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>1.668253968253968</v>
       </c>
-      <c r="G21" t="n">
+      <c r="H21" t="n">
         <v>99.9682</v>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>91.2</v>
       </c>
-      <c r="I21" t="n">
+      <c r="J21" t="n">
         <v>68.8</v>
       </c>
     </row>
@@ -1074,18 +1139,21 @@
         <v>75.7</v>
       </c>
       <c r="E22" t="n">
+        <v>80.40000000000001</v>
+      </c>
+      <c r="F22" t="n">
         <v>4.634166666666666</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>1.465833333333334</v>
       </c>
-      <c r="G22" t="n">
+      <c r="H22" t="n">
         <v>101.2842</v>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>92.09999999999999</v>
       </c>
-      <c r="I22" t="n">
+      <c r="J22" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1103,18 +1171,21 @@
         <v>75.7</v>
       </c>
       <c r="E23" t="n">
+        <v>80.7</v>
+      </c>
+      <c r="F23" t="n">
         <v>4.736666666666667</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>1.415</v>
       </c>
-      <c r="G23" t="n">
+      <c r="H23" t="n">
         <v>99.2963</v>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>93</v>
       </c>
-      <c r="I23" t="n">
+      <c r="J23" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1132,18 +1203,21 @@
         <v>75.59999999999999</v>
       </c>
       <c r="E24" t="n">
+        <v>81.40000000000001</v>
+      </c>
+      <c r="F24" t="n">
         <v>4.558333333333334</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>1.613333333333334</v>
       </c>
-      <c r="G24" t="n">
+      <c r="H24" t="n">
         <v>99.4624</v>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>94.09999999999999</v>
       </c>
-      <c r="I24" t="n">
+      <c r="J24" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1161,18 +1235,21 @@
         <v>75.09999999999999</v>
       </c>
       <c r="E25" t="n">
+        <v>81.59999999999999</v>
+      </c>
+      <c r="F25" t="n">
         <v>4.996666666666667</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>1.415</v>
       </c>
-      <c r="G25" t="n">
+      <c r="H25" t="n">
         <v>97.19410000000001</v>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>95.09999999999999</v>
       </c>
-      <c r="I25" t="n">
+      <c r="J25" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1190,18 +1267,21 @@
         <v>73.8</v>
       </c>
       <c r="E26" t="n">
+        <v>82.2</v>
+      </c>
+      <c r="F26" t="n">
         <v>4.965</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1.154166666666667</v>
       </c>
-      <c r="G26" t="n">
+      <c r="H26" t="n">
         <v>95.6559</v>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>96.2</v>
       </c>
-      <c r="I26" t="n">
+      <c r="J26" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1219,18 +1299,21 @@
         <v>75.90000000000001</v>
       </c>
       <c r="E27" t="n">
+        <v>82.5</v>
+      </c>
+      <c r="F27" t="n">
         <v>4.8825</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>1.165</v>
       </c>
-      <c r="G27" t="n">
+      <c r="H27" t="n">
         <v>93.4029</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>97.2</v>
       </c>
-      <c r="I27" t="n">
+      <c r="J27" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1248,18 +1331,21 @@
         <v>77.5</v>
       </c>
       <c r="E28" t="n">
+        <v>83</v>
+      </c>
+      <c r="F28" t="n">
         <v>3.963333333333333</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>1.515833333333333</v>
       </c>
-      <c r="G28" t="n">
+      <c r="H28" t="n">
         <v>92.6571</v>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>98.5</v>
       </c>
-      <c r="I28" t="n">
+      <c r="J28" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1277,18 +1363,21 @@
         <v>78.3</v>
       </c>
       <c r="E29" t="n">
+        <v>83.3</v>
+      </c>
+      <c r="F29" t="n">
         <v>3.425</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>1.845833333333333</v>
       </c>
-      <c r="G29" t="n">
+      <c r="H29" t="n">
         <v>93.12309999999999</v>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>99.59999999999999</v>
       </c>
-      <c r="I29" t="n">
+      <c r="J29" t="n">
         <v>67.40000000000001</v>
       </c>
     </row>
@@ -1306,18 +1395,21 @@
         <v>78.7</v>
       </c>
       <c r="E30" t="n">
+        <v>83.40000000000001</v>
+      </c>
+      <c r="F30" t="n">
         <v>3.483333333333333</v>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>1.695833333333334</v>
       </c>
-      <c r="G30" t="n">
+      <c r="H30" t="n">
         <v>93.03</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>100.5</v>
       </c>
-      <c r="I30" t="n">
+      <c r="J30" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1335,18 +1427,21 @@
         <v>78.59999999999999</v>
       </c>
       <c r="E31" t="n">
+        <v>83.90000000000001</v>
+      </c>
+      <c r="F31" t="n">
         <v>2.750833333333333</v>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>1.780833333333333</v>
       </c>
-      <c r="G31" t="n">
+      <c r="H31" t="n">
         <v>91.56780000000001</v>
       </c>
-      <c r="H31" t="n">
+      <c r="I31" t="n">
         <v>101.5</v>
       </c>
-      <c r="I31" t="n">
+      <c r="J31" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1364,18 +1459,21 @@
         <v>80.8</v>
       </c>
       <c r="E32" t="n">
+        <v>84.7</v>
+      </c>
+      <c r="F32" t="n">
         <v>2.661666666666667</v>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>1.646666666666667</v>
       </c>
-      <c r="G32" t="n">
+      <c r="H32" t="n">
         <v>93.3948</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>102.4</v>
       </c>
-      <c r="I32" t="n">
+      <c r="J32" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1393,18 +1491,21 @@
         <v>81.40000000000001</v>
       </c>
       <c r="E33" t="n">
+        <v>84.90000000000001</v>
+      </c>
+      <c r="F33" t="n">
         <v>2.624166666666667</v>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>1.2775</v>
       </c>
-      <c r="G33" t="n">
+      <c r="H33" t="n">
         <v>93.666</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>103.3</v>
       </c>
-      <c r="I33" t="n">
+      <c r="J33" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1422,18 +1523,21 @@
         <v>81.2</v>
       </c>
       <c r="E34" t="n">
+        <v>85.09999999999999</v>
+      </c>
+      <c r="F34" t="n">
         <v>2.798333333333333</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>1.0375</v>
       </c>
-      <c r="G34" t="n">
+      <c r="H34" t="n">
         <v>95.6544</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>104</v>
       </c>
-      <c r="I34" t="n">
+      <c r="J34" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1450,15 +1554,22 @@
       <c r="D35" t="n">
         <v>82.2</v>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr"/>
+      <c r="E35" t="n">
+        <v>85.40000000000001</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2.673333333333333</v>
+      </c>
       <c r="G35" t="n">
+        <v>1.190833333333334</v>
+      </c>
+      <c r="H35" t="n">
         <v>96.8764</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>105</v>
       </c>
-      <c r="I35" t="n">
+      <c r="J35" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1475,15 +1586,22 @@
       <c r="D36" t="n">
         <v>83.8</v>
       </c>
-      <c r="E36" t="inlineStr"/>
-      <c r="F36" t="inlineStr"/>
+      <c r="E36" t="n">
+        <v>86.40000000000001</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2.669333333333334</v>
+      </c>
       <c r="G36" t="n">
+        <v>1.243333333333333</v>
+      </c>
+      <c r="H36" t="n">
         <v>99.95399999999999</v>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>105.7</v>
       </c>
-      <c r="I36" t="n">
+      <c r="J36" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1501,18 +1619,21 @@
         <v>85.09999999999999</v>
       </c>
       <c r="E37" t="n">
+        <v>86.90000000000001</v>
+      </c>
+      <c r="F37" t="n">
         <v>2.731</v>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>0.993</v>
       </c>
-      <c r="G37" t="n">
+      <c r="H37" t="n">
         <v>100.7972</v>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>106.4</v>
       </c>
-      <c r="I37" t="n">
+      <c r="J37" t="n">
         <v>67.2</v>
       </c>
     </row>
@@ -1530,18 +1651,21 @@
         <v>86.5</v>
       </c>
       <c r="E38" t="n">
+        <v>87.40000000000001</v>
+      </c>
+      <c r="F38" t="n">
         <v>2.699</v>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>0.8596666666666667</v>
       </c>
-      <c r="G38" t="n">
+      <c r="H38" t="n">
         <v>102.2539</v>
       </c>
-      <c r="H38" t="n">
+      <c r="I38" t="n">
         <v>107</v>
       </c>
-      <c r="I38" t="n">
+      <c r="J38" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1559,18 +1683,21 @@
         <v>88.09999999999999</v>
       </c>
       <c r="E39" t="n">
+        <v>87.59999999999999</v>
+      </c>
+      <c r="F39" t="n">
         <v>2.685</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>0.7223333333333334</v>
       </c>
-      <c r="G39" t="n">
+      <c r="H39" t="n">
         <v>102.9975</v>
       </c>
-      <c r="H39" t="n">
+      <c r="I39" t="n">
         <v>107.5</v>
       </c>
-      <c r="I39" t="n">
+      <c r="J39" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1588,18 +1715,21 @@
         <v>89.2</v>
       </c>
       <c r="E40" t="n">
+        <v>88.09999999999999</v>
+      </c>
+      <c r="F40" t="n">
         <v>2.582666666666666</v>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>0.8186666666666667</v>
       </c>
-      <c r="G40" t="n">
+      <c r="H40" t="n">
         <v>104.8988</v>
       </c>
-      <c r="H40" t="n">
+      <c r="I40" t="n">
         <v>108.3</v>
       </c>
-      <c r="I40" t="n">
+      <c r="J40" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1617,18 +1747,21 @@
         <v>89.3</v>
       </c>
       <c r="E41" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="F41" t="n">
         <v>2.446</v>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>0.9476666666666667</v>
       </c>
-      <c r="G41" t="n">
+      <c r="H41" t="n">
         <v>106.3573</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>108.9</v>
       </c>
-      <c r="I41" t="n">
+      <c r="J41" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1646,18 +1779,21 @@
         <v>90</v>
       </c>
       <c r="E42" t="n">
+        <v>88.90000000000001</v>
+      </c>
+      <c r="F42" t="n">
         <v>1.955666666666667</v>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>0.9246666666666666</v>
       </c>
-      <c r="G42" t="n">
+      <c r="H42" t="n">
         <v>110.5975</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>109.2</v>
       </c>
-      <c r="I42" t="n">
+      <c r="J42" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1675,18 +1811,21 @@
         <v>89.8</v>
       </c>
       <c r="E43" t="n">
+        <v>89.3</v>
+      </c>
+      <c r="F43" t="n">
         <v>1.942666666666667</v>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>1.101333333333333</v>
       </c>
-      <c r="G43" t="n">
+      <c r="H43" t="n">
         <v>112.3251</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>109.6</v>
       </c>
-      <c r="I43" t="n">
+      <c r="J43" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1704,18 +1843,21 @@
         <v>92.40000000000001</v>
       </c>
       <c r="E44" t="n">
+        <v>89.90000000000001</v>
+      </c>
+      <c r="F44" t="n">
         <v>1.881666666666667</v>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>1.35</v>
       </c>
-      <c r="G44" t="n">
+      <c r="H44" t="n">
         <v>112.0823</v>
       </c>
-      <c r="H44" t="n">
+      <c r="I44" t="n">
         <v>109.9</v>
       </c>
-      <c r="I44" t="n">
+      <c r="J44" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1733,18 +1875,21 @@
         <v>92.59999999999999</v>
       </c>
       <c r="E45" t="n">
+        <v>90.2</v>
+      </c>
+      <c r="F45" t="n">
         <v>1.948666666666667</v>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>1.578666666666667</v>
       </c>
-      <c r="G45" t="n">
+      <c r="H45" t="n">
         <v>112.1175</v>
       </c>
-      <c r="H45" t="n">
+      <c r="I45" t="n">
         <v>110.1</v>
       </c>
-      <c r="I45" t="n">
+      <c r="J45" t="n">
         <v>67.5</v>
       </c>
     </row>
@@ -1762,18 +1907,21 @@
         <v>94.3</v>
       </c>
       <c r="E46" t="n">
+        <v>90</v>
+      </c>
+      <c r="F46" t="n">
         <v>1.904</v>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>1.901666666666667</v>
       </c>
-      <c r="G46" t="n">
+      <c r="H46" t="n">
         <v>113.9318</v>
       </c>
-      <c r="H46" t="n">
+      <c r="I46" t="n">
         <v>110.2</v>
       </c>
-      <c r="I46" t="n">
+      <c r="J46" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1791,18 +1939,21 @@
         <v>93.7</v>
       </c>
       <c r="E47" t="n">
+        <v>90</v>
+      </c>
+      <c r="F47" t="n">
         <v>1.729333333333334</v>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>1.402666666666667</v>
       </c>
-      <c r="G47" t="n">
+      <c r="H47" t="n">
         <v>114.7994</v>
       </c>
-      <c r="H47" t="n">
+      <c r="I47" t="n">
         <v>110.4</v>
       </c>
-      <c r="I47" t="n">
+      <c r="J47" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1820,18 +1971,21 @@
         <v>93.3</v>
       </c>
       <c r="E48" t="n">
+        <v>90.3</v>
+      </c>
+      <c r="F48" t="n">
         <v>1.522333333333333</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>1.137666666666667</v>
       </c>
-      <c r="G48" t="n">
+      <c r="H48" t="n">
         <v>118.9093</v>
       </c>
-      <c r="H48" t="n">
+      <c r="I48" t="n">
         <v>110.7</v>
       </c>
-      <c r="I48" t="n">
+      <c r="J48" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1849,18 +2003,21 @@
         <v>94</v>
       </c>
       <c r="E49" t="n">
+        <v>90.59999999999999</v>
+      </c>
+      <c r="F49" t="n">
         <v>1.745</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>1.203666666666667</v>
       </c>
-      <c r="G49" t="n">
+      <c r="H49" t="n">
         <v>120.9811</v>
       </c>
-      <c r="H49" t="n">
+      <c r="I49" t="n">
         <v>110.8</v>
       </c>
-      <c r="I49" t="n">
+      <c r="J49" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1878,18 +2035,21 @@
         <v>93.59999999999999</v>
       </c>
       <c r="E50" t="n">
+        <v>90.8</v>
+      </c>
+      <c r="F50" t="n">
         <v>1.815333333333333</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>0.976</v>
       </c>
-      <c r="G50" t="n">
+      <c r="H50" t="n">
         <v>123.1156</v>
       </c>
-      <c r="H50" t="n">
+      <c r="I50" t="n">
         <v>110.9</v>
       </c>
-      <c r="I50" t="n">
+      <c r="J50" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1907,18 +2067,21 @@
         <v>94.90000000000001</v>
       </c>
       <c r="E51" t="n">
+        <v>91.09999999999999</v>
+      </c>
+      <c r="F51" t="n">
         <v>1.661</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>1.037333333333333</v>
       </c>
-      <c r="G51" t="n">
+      <c r="H51" t="n">
         <v>122.0914</v>
       </c>
-      <c r="H51" t="n">
+      <c r="I51" t="n">
         <v>111.1</v>
       </c>
-      <c r="I51" t="n">
+      <c r="J51" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1936,18 +2099,21 @@
         <v>96</v>
       </c>
       <c r="E52" t="n">
+        <v>91.40000000000001</v>
+      </c>
+      <c r="F52" t="n">
         <v>1.816666666666667</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>0.8909999999999999</v>
       </c>
-      <c r="G52" t="n">
+      <c r="H52" t="n">
         <v>122.4909</v>
       </c>
-      <c r="H52" t="n">
+      <c r="I52" t="n">
         <v>111.3</v>
       </c>
-      <c r="I52" t="n">
+      <c r="J52" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1965,18 +2131,21 @@
         <v>96.3</v>
       </c>
       <c r="E53" t="n">
+        <v>91.90000000000001</v>
+      </c>
+      <c r="F53" t="n">
         <v>1.863666666666667</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>0.735</v>
       </c>
-      <c r="G53" t="n">
+      <c r="H53" t="n">
         <v>121.1208</v>
       </c>
-      <c r="H53" t="n">
+      <c r="I53" t="n">
         <v>111.6</v>
       </c>
-      <c r="I53" t="n">
+      <c r="J53" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -1994,18 +2163,21 @@
         <v>98.8</v>
       </c>
       <c r="E54" t="n">
+        <v>92.3</v>
+      </c>
+      <c r="F54" t="n">
         <v>1.975</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>0.7260000000000001</v>
       </c>
-      <c r="G54" t="n">
+      <c r="H54" t="n">
         <v>119.8688</v>
       </c>
-      <c r="H54" t="n">
+      <c r="I54" t="n">
         <v>111.8</v>
       </c>
-      <c r="I54" t="n">
+      <c r="J54" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2023,18 +2195,21 @@
         <v>99.3</v>
       </c>
       <c r="E55" t="n">
+        <v>92.7</v>
+      </c>
+      <c r="F55" t="n">
         <v>2.048666666666666</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>0.7756666666666666</v>
       </c>
-      <c r="G55" t="n">
+      <c r="H55" t="n">
         <v>117.5375</v>
       </c>
-      <c r="H55" t="n">
+      <c r="I55" t="n">
         <v>111.8</v>
       </c>
-      <c r="I55" t="n">
+      <c r="J55" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2052,18 +2227,21 @@
         <v>99.2</v>
       </c>
       <c r="E56" t="n">
+        <v>93.3</v>
+      </c>
+      <c r="F56" t="n">
         <v>2.014666666666667</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>0.8623333333333333</v>
       </c>
-      <c r="G56" t="n">
+      <c r="H56" t="n">
         <v>114.1473</v>
       </c>
-      <c r="H56" t="n">
+      <c r="I56" t="n">
         <v>112</v>
       </c>
-      <c r="I56" t="n">
+      <c r="J56" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2081,18 +2259,21 @@
         <v>99.90000000000001</v>
       </c>
       <c r="E57" t="n">
+        <v>93.8</v>
+      </c>
+      <c r="F57" t="n">
         <v>1.995</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>0.884</v>
       </c>
-      <c r="G57" t="n">
+      <c r="H57" t="n">
         <v>110.7228</v>
       </c>
-      <c r="H57" t="n">
+      <c r="I57" t="n">
         <v>112.2</v>
       </c>
-      <c r="I57" t="n">
+      <c r="J57" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2110,18 +2291,21 @@
         <v>100.6</v>
       </c>
       <c r="E58" t="n">
+        <v>94</v>
+      </c>
+      <c r="F58" t="n">
         <v>1.725666666666666</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>0.9833333333333334</v>
       </c>
-      <c r="G58" t="n">
+      <c r="H58" t="n">
         <v>109.2373</v>
       </c>
-      <c r="H58" t="n">
+      <c r="I58" t="n">
         <v>112.3</v>
       </c>
-      <c r="I58" t="n">
+      <c r="J58" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2139,18 +2323,21 @@
         <v>101.5</v>
       </c>
       <c r="E59" t="n">
+        <v>94.5</v>
+      </c>
+      <c r="F59" t="n">
         <v>1.233333333333333</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>0.8083333333333335</v>
       </c>
-      <c r="G59" t="n">
+      <c r="H59" t="n">
         <v>111.3297</v>
       </c>
-      <c r="H59" t="n">
+      <c r="I59" t="n">
         <v>112.3</v>
       </c>
-      <c r="I59" t="n">
+      <c r="J59" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2168,18 +2355,21 @@
         <v>102.5</v>
       </c>
       <c r="E60" t="n">
+        <v>94.90000000000001</v>
+      </c>
+      <c r="F60" t="n">
         <v>0.8223333333333334</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>0.8046666666666668</v>
       </c>
-      <c r="G60" t="n">
+      <c r="H60" t="n">
         <v>114.8865</v>
       </c>
-      <c r="H60" t="n">
+      <c r="I60" t="n">
         <v>112.4</v>
       </c>
-      <c r="I60" t="n">
+      <c r="J60" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2197,18 +2387,21 @@
         <v>103</v>
       </c>
       <c r="E61" t="n">
+        <v>95.40000000000001</v>
+      </c>
+      <c r="F61" t="n">
         <v>0.769</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>0.8523333333333332</v>
       </c>
-      <c r="G61" t="n">
+      <c r="H61" t="n">
         <v>116.3274</v>
       </c>
-      <c r="H61" t="n">
+      <c r="I61" t="n">
         <v>112.4</v>
       </c>
-      <c r="I61" t="n">
+      <c r="J61" t="n">
         <v>66.2</v>
       </c>
     </row>
@@ -2226,18 +2419,21 @@
         <v>102.9</v>
       </c>
       <c r="E62" t="n">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="F62" t="n">
         <v>0.6153333333333334</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>0.9386666666666666</v>
       </c>
-      <c r="G62" t="n">
+      <c r="H62" t="n">
         <v>116.4502</v>
       </c>
-      <c r="H62" t="n">
+      <c r="I62" t="n">
         <v>112.5</v>
       </c>
-      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2253,18 +2449,21 @@
         <v>100</v>
       </c>
       <c r="E63" t="n">
+        <v>95.5</v>
+      </c>
+      <c r="F63" t="n">
         <v>0.2443333333333333</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>1.278666666666667</v>
       </c>
-      <c r="G63" t="n">
+      <c r="H63" t="n">
         <v>115.5269</v>
       </c>
-      <c r="H63" t="n">
+      <c r="I63" t="n">
         <v>111</v>
       </c>
-      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2280,18 +2479,21 @@
         <v>100.3</v>
       </c>
       <c r="E64" t="n">
+        <v>95.59999999999999</v>
+      </c>
+      <c r="F64" t="n">
         <v>0.2513333333333334</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>0.664</v>
       </c>
-      <c r="G64" t="n">
+      <c r="H64" t="n">
         <v>118.0338</v>
       </c>
-      <c r="H64" t="n">
+      <c r="I64" t="n">
         <v>110.8</v>
       </c>
-      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2307,16 +2509,19 @@
         <v>100.3</v>
       </c>
       <c r="E65" t="n">
+        <v>96</v>
+      </c>
+      <c r="F65" t="n">
         <v>0.1093333333333333</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>0.533</v>
       </c>
-      <c r="G65" t="inlineStr"/>
-      <c r="H65" t="n">
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="n">
         <v>110.9</v>
       </c>
-      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fix: use MP surprises as the correct shock
</commit_message>
<xml_diff>
--- a/data/quarterly_data_AUS.xlsx
+++ b/data/quarterly_data_AUS.xlsx
@@ -642,7 +642,7 @@
         <v>72.90000000000001</v>
       </c>
       <c r="J6" t="n">
-        <v>68.3</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="7">
@@ -674,7 +674,7 @@
         <v>73.5</v>
       </c>
       <c r="J7" t="n">
-        <v>68.3</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="8">
@@ -706,7 +706,7 @@
         <v>74.3</v>
       </c>
       <c r="J8" t="n">
-        <v>68.3</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="9">
@@ -738,7 +738,7 @@
         <v>75</v>
       </c>
       <c r="J9" t="n">
-        <v>68.3</v>
+        <v>69.3</v>
       </c>
     </row>
     <row r="10">
@@ -898,7 +898,7 @@
         <v>81.40000000000001</v>
       </c>
       <c r="J14" t="n">
-        <v>68.8</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="15">
@@ -930,7 +930,7 @@
         <v>83.3</v>
       </c>
       <c r="J15" t="n">
-        <v>68.8</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="16">
@@ -962,7 +962,7 @@
         <v>85</v>
       </c>
       <c r="J16" t="n">
-        <v>68.8</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="17">
@@ -994,7 +994,7 @@
         <v>86.7</v>
       </c>
       <c r="J17" t="n">
-        <v>68.8</v>
+        <v>68.3</v>
       </c>
     </row>
     <row r="18">
@@ -1154,7 +1154,7 @@
         <v>92.09999999999999</v>
       </c>
       <c r="J22" t="n">
-        <v>67.40000000000001</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="23">
@@ -1186,7 +1186,7 @@
         <v>93</v>
       </c>
       <c r="J23" t="n">
-        <v>67.40000000000001</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="24">
@@ -1218,7 +1218,7 @@
         <v>94.09999999999999</v>
       </c>
       <c r="J24" t="n">
-        <v>67.40000000000001</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="25">
@@ -1250,7 +1250,7 @@
         <v>95.09999999999999</v>
       </c>
       <c r="J25" t="n">
-        <v>67.40000000000001</v>
+        <v>68.8</v>
       </c>
     </row>
     <row r="26">
@@ -1410,7 +1410,7 @@
         <v>100.5</v>
       </c>
       <c r="J30" t="n">
-        <v>67.2</v>
+        <v>67.40000000000001</v>
       </c>
     </row>
     <row r="31">
@@ -1442,7 +1442,7 @@
         <v>101.5</v>
       </c>
       <c r="J31" t="n">
-        <v>67.2</v>
+        <v>67.40000000000001</v>
       </c>
     </row>
     <row r="32">
@@ -1474,7 +1474,7 @@
         <v>102.4</v>
       </c>
       <c r="J32" t="n">
-        <v>67.2</v>
+        <v>67.40000000000001</v>
       </c>
     </row>
     <row r="33">
@@ -1506,7 +1506,7 @@
         <v>103.3</v>
       </c>
       <c r="J33" t="n">
-        <v>67.2</v>
+        <v>67.40000000000001</v>
       </c>
     </row>
     <row r="34">
@@ -1666,7 +1666,7 @@
         <v>107</v>
       </c>
       <c r="J38" t="n">
-        <v>67.5</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="39">
@@ -1698,7 +1698,7 @@
         <v>107.5</v>
       </c>
       <c r="J39" t="n">
-        <v>67.5</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="40">
@@ -1730,7 +1730,7 @@
         <v>108.3</v>
       </c>
       <c r="J40" t="n">
-        <v>67.5</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="41">
@@ -1762,7 +1762,7 @@
         <v>108.9</v>
       </c>
       <c r="J41" t="n">
-        <v>67.5</v>
+        <v>67.2</v>
       </c>
     </row>
     <row r="42">
@@ -1922,7 +1922,7 @@
         <v>110.2</v>
       </c>
       <c r="J46" t="n">
-        <v>66.2</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="47">
@@ -1954,7 +1954,7 @@
         <v>110.4</v>
       </c>
       <c r="J47" t="n">
-        <v>66.2</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="48">
@@ -1986,7 +1986,7 @@
         <v>110.7</v>
       </c>
       <c r="J48" t="n">
-        <v>66.2</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="49">
@@ -2018,7 +2018,7 @@
         <v>110.8</v>
       </c>
       <c r="J49" t="n">
-        <v>66.2</v>
+        <v>67.5</v>
       </c>
     </row>
     <row r="50">
@@ -2433,7 +2433,9 @@
       <c r="I62" t="n">
         <v>112.5</v>
       </c>
-      <c r="J62" t="inlineStr"/>
+      <c r="J62" t="n">
+        <v>66.2</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -2463,7 +2465,9 @@
       <c r="I63" t="n">
         <v>111</v>
       </c>
-      <c r="J63" t="inlineStr"/>
+      <c r="J63" t="n">
+        <v>66.2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -2493,7 +2497,9 @@
       <c r="I64" t="n">
         <v>110.8</v>
       </c>
-      <c r="J64" t="inlineStr"/>
+      <c r="J64" t="n">
+        <v>66.2</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -2521,7 +2527,9 @@
       <c r="I65" t="n">
         <v>110.9</v>
       </c>
-      <c r="J65" t="inlineStr"/>
+      <c r="J65" t="n">
+        <v>66.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>